<commit_message>
Adicionando o commit final
</commit_message>
<xml_diff>
--- a/dashboard/dim-localizacao.xlsx
+++ b/dashboard/dim-localizacao.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="RM552628.DIM_LOCALIZACAO" r:id="rId3" sheetId="1"/>
+    <sheet name="RM553315.DIM_LOCALIZACAO" r:id="rId3" sheetId="1"/>
     <sheet name="SQL" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
@@ -18,7 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm AM/PM"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11.0"/>
@@ -52,11 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -66,7 +71,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C551"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -178,7 +183,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MaceiÃ³</t>
+          <t>Maceio</t>
         </is>
       </c>
     </row>
@@ -208,7 +213,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -223,7 +228,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -238,7 +243,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -253,7 +258,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -268,7 +273,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -283,7 +288,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -298,7 +303,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -313,7 +318,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Palmeira dos Ã�ndios</t>
+          <t>Palmeira dos Indios</t>
         </is>
       </c>
     </row>
@@ -328,7 +333,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MacapÃ¡</t>
+          <t>Macapa</t>
         </is>
       </c>
     </row>
@@ -658,7 +663,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VitÃ³ria da Conquista</t>
+          <t>Vitoria da Conquista</t>
         </is>
       </c>
     </row>
@@ -673,7 +678,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -688,7 +693,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -703,7 +708,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -718,7 +723,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -733,7 +738,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -748,7 +753,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -763,7 +768,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -778,7 +783,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -793,7 +798,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -808,7 +813,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -823,7 +828,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -838,7 +843,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -853,7 +858,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -868,7 +873,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -883,7 +888,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -898,7 +903,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -913,7 +918,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -928,7 +933,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -943,7 +948,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -958,7 +963,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -973,7 +978,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -988,7 +993,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1008,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1018,7 +1023,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1038,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1053,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1068,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>IlhÃ©us</t>
+          <t>Ilheus</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1458,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1473,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1488,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1498,7 +1503,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1518,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1533,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1548,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1563,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1578,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1593,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1603,7 +1608,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1618,7 +1623,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1633,7 +1638,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1653,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1663,7 +1668,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1678,7 +1683,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1698,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1713,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1723,7 +1728,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1743,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>BrasÃ­lia</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1758,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>VitÃ³ria</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
@@ -1978,7 +1983,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>GoiÃ¢nia</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1998,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Aparecida de GoiÃ¢nia</t>
+          <t>Aparecida de Goiania</t>
         </is>
       </c>
     </row>
@@ -2008,7 +2013,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2023,7 +2028,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2043,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2053,7 +2058,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2068,7 +2073,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2083,7 +2088,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2103,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2118,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2133,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2143,7 +2148,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2158,7 +2163,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2173,7 +2178,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2193,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2203,7 +2208,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2218,7 +2223,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2238,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2248,7 +2253,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2268,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2278,7 +2283,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2293,7 +2298,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2308,7 +2313,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2328,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2343,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>AnÃ¡polis</t>
+          <t>Anapolis</t>
         </is>
       </c>
     </row>
@@ -2353,7 +2358,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>SÃ£o LuÃ­s</t>
+          <t>Sao Luis</t>
         </is>
       </c>
     </row>
@@ -2578,7 +2583,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>CuiabÃ¡</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2598,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>VÃ¡rzea Grande</t>
+          <t>Varzea Grande</t>
         </is>
       </c>
     </row>
@@ -2608,7 +2613,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2623,7 +2628,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2643,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2658,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2668,7 +2673,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2688,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2703,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2718,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2728,7 +2733,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2743,7 +2748,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2758,7 +2763,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2778,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2793,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>RondonÃ³polis</t>
+          <t>Rondonopolis</t>
         </is>
       </c>
     </row>
@@ -2833,7 +2838,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2848,7 +2853,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2863,7 +2868,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2878,7 +2883,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2898,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2908,7 +2913,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2923,7 +2928,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2938,7 +2943,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2958,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2968,7 +2973,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2983,7 +2988,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -2998,7 +3003,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -3013,7 +3018,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>TrÃªs Lagoas</t>
+          <t>Tres Lagoas</t>
         </is>
       </c>
     </row>
@@ -3043,7 +3048,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>UberlÃ¢ndia</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
@@ -3778,7 +3783,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>BelÃ©m</t>
+          <t>Belem</t>
         </is>
       </c>
     </row>
@@ -3808,7 +3813,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3823,7 +3828,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3838,7 +3843,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3853,7 +3858,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3868,7 +3873,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3888,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3898,7 +3903,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3913,7 +3918,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3928,7 +3933,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3943,7 +3948,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3958,7 +3963,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3973,7 +3978,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -3988,7 +3993,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4003,7 +4008,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4018,7 +4023,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4033,7 +4038,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4053,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4063,7 +4068,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>SantarÃ©m</t>
+          <t>Santarem</t>
         </is>
       </c>
     </row>
@@ -4078,7 +4083,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>JoÃ£o Pessoa</t>
+          <t>Joao Pessoa</t>
         </is>
       </c>
     </row>
@@ -4333,7 +4338,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>MaringÃ¡</t>
+          <t>Maringa</t>
         </is>
       </c>
     </row>
@@ -4768,7 +4773,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>JaboatÃ£o dos Guararapes</t>
+          <t>Jaboatao dos Guararapes</t>
         </is>
       </c>
     </row>
@@ -5143,7 +5148,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>ParnaÃ­ba</t>
+          <t>Parnaiba</t>
         </is>
       </c>
     </row>
@@ -5293,7 +5298,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>NiterÃ³i</t>
+          <t>Niteroi</t>
         </is>
       </c>
     </row>
@@ -5308,7 +5313,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>SÃ£o GonÃ§alo</t>
+          <t>Sao Goncalo</t>
         </is>
       </c>
     </row>
@@ -5893,7 +5898,7 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>MossorÃ³</t>
+          <t>Mossoro</t>
         </is>
       </c>
     </row>
@@ -6568,7 +6573,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>Ji-ParanÃ¡</t>
+          <t>Ji Parana</t>
         </is>
       </c>
     </row>
@@ -6718,7 +6723,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>RorainÃ³polis</t>
+          <t>Rorainopolis</t>
         </is>
       </c>
     </row>
@@ -6733,7 +6738,7 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>CaracaraÃ­</t>
+          <t>Caracarai</t>
         </is>
       </c>
     </row>
@@ -6748,7 +6753,7 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>CaracaraÃ­</t>
+          <t>Caracarai</t>
         </is>
       </c>
     </row>
@@ -6763,7 +6768,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>CaracaraÃ­</t>
+          <t>Caracarai</t>
         </is>
       </c>
     </row>
@@ -6778,7 +6783,7 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>FlorianÃ³polis</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
@@ -6823,7 +6828,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6838,7 +6843,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6853,7 +6858,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6868,7 +6873,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6883,7 +6888,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6898,7 +6903,7 @@
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6913,7 +6918,7 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6928,7 +6933,7 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6943,7 +6948,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6958,7 +6963,7 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6973,7 +6978,7 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -6988,7 +6993,7 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7003,7 +7008,7 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7018,7 +7023,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7033,7 +7038,7 @@
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7048,7 +7053,7 @@
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7063,7 +7068,7 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7078,7 +7083,7 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7093,7 +7098,7 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7108,7 +7113,7 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7123,7 +7128,7 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7138,7 +7143,7 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>SÃ£o JosÃ©</t>
+          <t>Sao Jose</t>
         </is>
       </c>
     </row>
@@ -7153,7 +7158,7 @@
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>SÃ£o Paulo</t>
+          <t>Sao Paulo</t>
         </is>
       </c>
     </row>
@@ -7183,7 +7188,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>SÃ£o Bernardo do Campo</t>
+          <t>Sao Bernardo do Campo</t>
         </is>
       </c>
     </row>
@@ -7198,7 +7203,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7213,7 +7218,7 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7228,7 +7233,7 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7243,7 +7248,7 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7258,7 +7263,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7273,7 +7278,7 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7288,7 +7293,7 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7303,7 +7308,7 @@
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7318,7 +7323,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7333,7 +7338,7 @@
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7348,7 +7353,7 @@
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7363,7 +7368,7 @@
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7378,7 +7383,7 @@
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7393,7 +7398,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7408,7 +7413,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7423,7 +7428,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7438,7 +7443,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7453,7 +7458,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7468,7 +7473,7 @@
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7483,7 +7488,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7498,7 +7503,7 @@
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7513,7 +7518,7 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7528,7 +7533,7 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7543,7 +7548,7 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7558,7 +7563,7 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7573,7 +7578,7 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7588,7 +7593,7 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7603,7 +7608,7 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7618,7 +7623,7 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7633,7 +7638,7 @@
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7648,7 +7653,7 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7663,7 +7668,7 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7678,7 +7683,7 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7693,7 +7698,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7708,7 +7713,7 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7723,7 +7728,7 @@
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7738,7 +7743,7 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7753,7 +7758,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7768,7 +7773,7 @@
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7783,7 +7788,7 @@
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7798,7 +7803,7 @@
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7813,7 +7818,7 @@
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7828,7 +7833,7 @@
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7843,7 +7848,7 @@
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7858,7 +7863,7 @@
       </c>
       <c r="C519" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7873,7 +7878,7 @@
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7888,7 +7893,7 @@
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7903,7 +7908,7 @@
       </c>
       <c r="C522" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7918,7 +7923,7 @@
       </c>
       <c r="C523" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7933,7 +7938,7 @@
       </c>
       <c r="C524" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7948,7 +7953,7 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7963,7 +7968,7 @@
       </c>
       <c r="C526" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7978,7 +7983,7 @@
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -7993,7 +7998,7 @@
       </c>
       <c r="C528" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -8008,7 +8013,7 @@
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -8023,7 +8028,7 @@
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -8038,7 +8043,7 @@
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>Santo AndrÃ©</t>
+          <t>Santo Andre</t>
         </is>
       </c>
     </row>
@@ -8218,7 +8223,7 @@
       </c>
       <c r="C543" t="inlineStr">
         <is>
-          <t>AraguaÃ­na</t>
+          <t>Araguaina</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8354,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8358,7 +8363,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>select SEQ_ENDERECO_CLIENTE SEQ_ENDERECO_CLIENTE, ESTADO ESTADO, CIDADE CIDADE from (select * from "RM552628"."DIM_LOCALIZACAO")</t>
+          <t>select SEQ_ENDERECO_CLIENTE SEQ_ENDERECO_CLIENTE, ESTADO ESTADO, CIDADE CIDADE from (select * from "RM553315"."DIM_LOCALIZACAO")</t>
         </is>
       </c>
     </row>

</xml_diff>